<commit_message>
api upload file excel customer old
</commit_message>
<xml_diff>
--- a/store/hoso/dulieu.xlsx
+++ b/store/hoso/dulieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THỰC TẬP 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76551177-F27E-4C5C-A4CC-10B8AD812104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9179A1BC-3EDE-4738-B91A-CC858CD18E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2970,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y306" sqref="Y306:Y334"/>
+    <sheetView tabSelected="1" topLeftCell="F309" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N320" sqref="N320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>